<commit_message>
updates with $location + update documentation
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\AngularJS-project\Ads\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -198,13 +198,22 @@
   </si>
   <si>
     <t>∞</t>
+  </si>
+  <si>
+    <t>Ventsislav</t>
+  </si>
+  <si>
+    <t>Ventsislav Yordanov</t>
+  </si>
+  <si>
+    <t>https://github.com/Venciity/AngularJS-project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +243,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -329,10 +346,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -360,6 +378,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,20 +402,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,44 +714,50 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="C7" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -752,12 +780,12 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
@@ -769,7 +797,9 @@
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -779,7 +809,9 @@
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
@@ -789,7 +821,9 @@
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -809,7 +843,9 @@
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -819,7 +855,9 @@
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
@@ -829,7 +867,9 @@
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -839,7 +879,9 @@
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -849,7 +891,9 @@
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -859,7 +903,9 @@
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
@@ -869,7 +915,9 @@
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -879,7 +927,9 @@
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
@@ -899,7 +949,9 @@
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
@@ -909,7 +961,9 @@
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
@@ -919,7 +973,9 @@
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
@@ -929,7 +985,9 @@
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
@@ -939,7 +997,9 @@
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
@@ -982,12 +1042,12 @@
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -1182,7 +1242,10 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update edit ad and edit profile
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -399,10 +399,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +753,11 @@
       <c r="B7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -1009,7 +1009,9 @@
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
@@ -1019,7 +1021,9 @@
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
@@ -1029,7 +1033,9 @@
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">

</xml_diff>

<commit_message>
add part of admin home view
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add delete ad by admin
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>https://github.com/Venciity/AngularJS-project</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1066,9 @@
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -1073,7 +1078,9 @@
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="7"/>
+      <c r="E35" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
@@ -1083,7 +1090,9 @@
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
@@ -1093,7 +1102,9 @@
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
@@ -1103,7 +1114,9 @@
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">

</xml_diff>

<commit_message>
add edit user profile by admin
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -692,7 +692,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1126,9 @@
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">

</xml_diff>

<commit_message>
add change user password
</commit_message>
<xml_diff>
--- a/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/Documentation/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -692,7 +692,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1138,9 @@
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">

</xml_diff>